<commit_message>
Add an effect size classification column
</commit_message>
<xml_diff>
--- a/Datos/article_data_master.xlsx
+++ b/Datos/article_data_master.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/MBP/Ponce Health Sciences University/Evidence computer-assisted reading interventions - Documentos/Datos/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1605" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{0F6C3925-34D1-5044-A170-5BFE297688CA}"/>
+  <xr:revisionPtr revIDLastSave="1642" documentId="11_E81672FC5CF8BA3067CC11F7F7A78F6A5450F117" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{229A5D32-C655-B445-9AF5-CE3F33068270}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="32000" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11000" yWindow="0" windowWidth="21000" windowHeight="18000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="881" uniqueCount="404">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="414">
   <si>
     <t>wV3t2Vi41UG_v9slVOJjbu3u5fMQrclPm0-s5s2WAKtUQ1FNTjZOUzAyMjY1RVNTTExEQ1paSk8wOCQlQCN0PWcu</t>
   </si>
@@ -517,9 +517,6 @@
     <t>Wilcoxon analyses were conducted because of sample size</t>
   </si>
   <si>
-    <t>Participants with difficulties in different skills received both interventions (i.e., training of their areas of difficulty and training on other areas), but the results presented here are only focused on the type of intervention, irrespective of the participant's difficulties.</t>
-  </si>
-  <si>
     <t>Many statistical analyses were conducted</t>
   </si>
   <si>
@@ -1278,6 +1275,39 @@
   </si>
   <si>
     <t>n2 = .04 - .159</t>
+  </si>
+  <si>
+    <t>Effect size classification</t>
+  </si>
+  <si>
+    <t>Large</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>medium to large</t>
+  </si>
+  <si>
+    <t>large</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Comprehension training: .52 - .88</t>
+  </si>
+  <si>
+    <t>Grapho-syllabic training: large, Comprehension training: medium to large</t>
+  </si>
+  <si>
+    <t>small to large</t>
+  </si>
+  <si>
+    <t>small to medium</t>
+  </si>
+  <si>
+    <t>Posttest: small to large, follow-up: small to large</t>
   </si>
 </sst>
 </file>
@@ -1350,7 +1380,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -1366,11 +1396,17 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="55">
+  <dxfs count="56">
     <dxf>
       <font>
         <strike val="0"/>
@@ -1385,27 +1421,15 @@
         <scheme val="none"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
+        <b val="0"/>
+        <i val="0"/>
         <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="12"/>
-        <color theme="1"/>
-        <name val="Times New Roman"/>
-        <family val="1"/>
-        <scheme val="none"/>
-      </font>
-      <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
-      <font>
-        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
         <outline val="0"/>
         <shadow val="0"/>
         <u val="none"/>
@@ -2267,6 +2291,38 @@
       <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <font>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Times New Roman"/>
+        <family val="1"/>
+        <scheme val="none"/>
+      </font>
+      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
@@ -2287,65 +2343,66 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA48DFE5-A6EC-48FC-85CA-4154DEEA6FCC}" name="Table1" displayName="Table1" ref="A1:BA23" totalsRowShown="0" headerRowDxfId="1" dataDxfId="0">
-  <autoFilter ref="A1:BA23" xr:uid="{F61FD2A4-1CA2-3C4C-BBCC-B5262A755B8C}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:BA23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{BA48DFE5-A6EC-48FC-85CA-4154DEEA6FCC}" name="Table1" displayName="Table1" ref="A1:BB23" totalsRowShown="0" headerRowDxfId="55" dataDxfId="54">
+  <autoFilter ref="A1:BB23" xr:uid="{F61FD2A4-1CA2-3C4C-BBCC-B5262A755B8C}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:BB23">
     <sortCondition ref="A1:A23"/>
   </sortState>
-  <tableColumns count="53">
-    <tableColumn id="1" xr3:uid="{0B078E7E-83E4-453C-8557-B689B2516465}" name="ID" dataDxfId="54"/>
-    <tableColumn id="6" xr3:uid="{3AD873ED-B3D7-417E-A6AB-800F1E5459F4}" name="Author" dataDxfId="53"/>
-    <tableColumn id="8" xr3:uid="{4044AAAA-9E80-4793-AC51-E5F5CD0694AD}" name="Year" dataDxfId="52"/>
-    <tableColumn id="9" xr3:uid="{8364FC52-A4F5-407C-918E-33C3CFAA4542}" name="Title" dataDxfId="51"/>
-    <tableColumn id="10" xr3:uid="{F5CA48F2-8F78-4303-B81F-A731AECB9DFA}" name="Purpose" dataDxfId="50"/>
-    <tableColumn id="11" xr3:uid="{AF745F93-691A-410F-9848-43E62584120C}" name="Cognitive processes to impact" dataDxfId="49"/>
-    <tableColumn id="5" xr3:uid="{F3021936-B951-5947-8D9A-D7DDA52C37DD}" name="Reading skills to impact" dataDxfId="48"/>
-    <tableColumn id="12" xr3:uid="{ED5FC934-5B38-4BA8-9AE2-91F922F96E30}" name="Reading skills to impact_coded" dataDxfId="47"/>
-    <tableColumn id="14" xr3:uid="{85807B29-1C14-4F47-B5D5-4AE5569A0A05}" name="Design" dataDxfId="46"/>
-    <tableColumn id="2" xr3:uid="{2B5A5073-6303-1046-A445-26BB37292EFE}" name="Design_coded" dataDxfId="45"/>
-    <tableColumn id="56" xr3:uid="{932A60C9-8B73-4E92-87A5-23592C00770D}" name="Inferred design" dataDxfId="44"/>
-    <tableColumn id="16" xr3:uid="{01B4398B-886B-4B39-9F7C-BB3550166D78}" name="Number of participants" dataDxfId="43"/>
-    <tableColumn id="17" xr3:uid="{45C5B1E8-14B1-4491-AEE9-F20EEC3E0F49}" name="Probabilistic sampling" dataDxfId="42"/>
-    <tableColumn id="19" xr3:uid="{51CA66B9-1DFA-464C-BC3B-6EA038A92C8A}" name="Grade" dataDxfId="41"/>
-    <tableColumn id="21" xr3:uid="{061D070E-4B42-4273-9AAD-4EC93B84AD81}" name="Age" dataDxfId="40"/>
-    <tableColumn id="22" xr3:uid="{31070516-608E-41E0-93C1-2CC77E80426F}" name="Language" dataDxfId="39"/>
-    <tableColumn id="23" xr3:uid="{C92854F5-2EF0-4285-B7F6-8C05B4A90195}" name="Session number" dataDxfId="38"/>
-    <tableColumn id="24" xr3:uid="{B30E45D7-CC2B-4FDC-81C4-AB4317E182CE}" name="Session duration" dataDxfId="37"/>
-    <tableColumn id="25" xr3:uid="{19C302C0-56F0-45E0-95EE-BCBDAF18F282}" name="sessions frequency" dataDxfId="36"/>
-    <tableColumn id="26" xr3:uid="{ACEA4A35-6C0A-4701-8F70-24864DBA8770}" name="Modality" dataDxfId="35"/>
-    <tableColumn id="27" xr3:uid="{A06FDE04-A553-4BEF-995A-31322B29A28C}" name="Participants in group modality" dataDxfId="34"/>
-    <tableColumn id="28" xr3:uid="{0FED9BC8-7DB8-4F8E-B677-DADF5940B6CC}" name="Supervision" dataDxfId="33"/>
-    <tableColumn id="29" xr3:uid="{4D548382-0ABC-4BD6-9A3D-78FCE85DCBC1}" name="Intervention name" dataDxfId="32"/>
-    <tableColumn id="30" xr3:uid="{63FCD5C3-B077-493B-B321-B0604366EB96}" name="Instruments to measure cognition" dataDxfId="31"/>
-    <tableColumn id="31" xr3:uid="{E3A52C0B-9BE7-4A14-93E7-C4247CE91B90}" name="Instruments to measure reading skills" dataDxfId="30"/>
-    <tableColumn id="32" xr3:uid="{0D56973D-C88D-40FE-A90F-B0AFB213AFDF}" name="Random assignment" dataDxfId="29"/>
-    <tableColumn id="33" xr3:uid="{ECFDDC08-D3B7-4CF9-AF2D-BA1AAE9641F6}" name="Assessment counterbalancing" dataDxfId="28"/>
-    <tableColumn id="34" xr3:uid="{EE5CE2B4-6D44-44A0-BC90-566EB9520766}" name="Variables for group balance" dataDxfId="27"/>
-    <tableColumn id="37" xr3:uid="{C28C160E-D7AE-41F1-9FB7-C3E66D709720}" name="Other methodological controls" dataDxfId="26"/>
-    <tableColumn id="38" xr3:uid="{2EA382FB-29FE-4AAB-A2D4-55C13414BFF5}" name="Descriptive statistics provided" dataDxfId="25"/>
-    <tableColumn id="39" xr3:uid="{09505FCD-0E9E-4883-A35E-0564AA34BA56}" name="Mean/Median" dataDxfId="24"/>
-    <tableColumn id="40" xr3:uid="{484DDF92-F6A0-4359-8958-DC5B1C8A3B0C}" name="Standard deviation" dataDxfId="23"/>
-    <tableColumn id="41" xr3:uid="{55D2984D-1B81-4C5D-887F-785B42549436}" name="Mean confidence interval" dataDxfId="22"/>
-    <tableColumn id="42" xr3:uid="{1C5ABDAC-5E8F-4586-AF3F-5CE38E434290}" name="Other descriptive statistics" dataDxfId="21"/>
-    <tableColumn id="57" xr3:uid="{C48DCD7B-4527-4E53-A3F7-E60E0ECEF558}" name="Comments about descriptive statistics" dataDxfId="20"/>
-    <tableColumn id="44" xr3:uid="{7A4931EC-DAB2-43FD-9563-B41C63AF994C}" name="Inferential statistics" dataDxfId="19"/>
-    <tableColumn id="45" xr3:uid="{04FD368E-6727-4A16-B432-6055946ADB4E}" name="Covariate" dataDxfId="18"/>
-    <tableColumn id="46" xr3:uid="{002B09FC-42A5-4B9E-B00B-4247469ED640}" name="Specific p-value provided" dataDxfId="17"/>
-    <tableColumn id="47" xr3:uid="{2491D4F3-A98E-4ED6-9CC0-5BEBA0AED5A2}" name="Effect size provided" dataDxfId="16"/>
-    <tableColumn id="48" xr3:uid="{ED100DE6-09FF-4604-99D6-73681EB7237F}" name="Mean difference confidence interval" dataDxfId="15"/>
-    <tableColumn id="49" xr3:uid="{51DB6773-4D14-4AE1-9DA6-3C452E8BD712}" name="Other statistical controls" dataDxfId="14"/>
-    <tableColumn id="58" xr3:uid="{5B74B444-7863-49DC-BECA-49FEE05F9984}" name="Comments inferential statistics" dataDxfId="13"/>
-    <tableColumn id="50" xr3:uid="{E36D3572-9344-404D-AEED-4C18E7A993EF}" name="Improved cognitive processes" dataDxfId="12"/>
-    <tableColumn id="51" xr3:uid="{2B520559-FCB3-4512-B091-68EA56AAEE21}" name="Cognitive processes that did not improve" dataDxfId="11"/>
-    <tableColumn id="52" xr3:uid="{1EA75320-37D8-4F15-940E-B6A10594C3A3}" name="Effect size cognition" dataDxfId="10"/>
-    <tableColumn id="59" xr3:uid="{D5BEAA29-1A8C-40F5-9AC8-5637860CE237}" name="Comments effect on cognition" dataDxfId="9"/>
-    <tableColumn id="3" xr3:uid="{05BA5D65-9865-E24C-8C24-D3F101DAAF39}" name="Improved reading skills" dataDxfId="8"/>
-    <tableColumn id="53" xr3:uid="{C933BD5B-B918-4F2D-B8F7-CD8E7A132A17}" name="Improved reading skills_coded" dataDxfId="7"/>
-    <tableColumn id="4" xr3:uid="{7FF23964-25F2-9E4E-A060-98AF4F47BE84}" name="Reading skills no improvement" dataDxfId="6"/>
-    <tableColumn id="54" xr3:uid="{F39DD7A1-CBC3-4AF0-B362-68FFD32F347B}" name="Reading skills no improvement_coded" dataDxfId="5"/>
-    <tableColumn id="55" xr3:uid="{A6F391AD-5850-47C2-9D08-4CFA06D01676}" name="Effect size reading skills" dataDxfId="4"/>
-    <tableColumn id="60" xr3:uid="{6050F297-C3B7-4DDE-A740-5139D8EAF8F5}" name="Comments effect on reading skills" dataDxfId="3"/>
-    <tableColumn id="61" xr3:uid="{C3B05082-6C97-4BD7-B093-5FB9EEC21E36}" name="General comments" dataDxfId="2"/>
+  <tableColumns count="54">
+    <tableColumn id="1" xr3:uid="{0B078E7E-83E4-453C-8557-B689B2516465}" name="ID" dataDxfId="53"/>
+    <tableColumn id="6" xr3:uid="{3AD873ED-B3D7-417E-A6AB-800F1E5459F4}" name="Author" dataDxfId="52"/>
+    <tableColumn id="8" xr3:uid="{4044AAAA-9E80-4793-AC51-E5F5CD0694AD}" name="Year" dataDxfId="51"/>
+    <tableColumn id="9" xr3:uid="{8364FC52-A4F5-407C-918E-33C3CFAA4542}" name="Title" dataDxfId="50"/>
+    <tableColumn id="10" xr3:uid="{F5CA48F2-8F78-4303-B81F-A731AECB9DFA}" name="Purpose" dataDxfId="49"/>
+    <tableColumn id="11" xr3:uid="{AF745F93-691A-410F-9848-43E62584120C}" name="Cognitive processes to impact" dataDxfId="48"/>
+    <tableColumn id="5" xr3:uid="{F3021936-B951-5947-8D9A-D7DDA52C37DD}" name="Reading skills to impact" dataDxfId="47"/>
+    <tableColumn id="12" xr3:uid="{ED5FC934-5B38-4BA8-9AE2-91F922F96E30}" name="Reading skills to impact_coded" dataDxfId="46"/>
+    <tableColumn id="14" xr3:uid="{85807B29-1C14-4F47-B5D5-4AE5569A0A05}" name="Design" dataDxfId="45"/>
+    <tableColumn id="2" xr3:uid="{2B5A5073-6303-1046-A445-26BB37292EFE}" name="Design_coded" dataDxfId="44"/>
+    <tableColumn id="56" xr3:uid="{932A60C9-8B73-4E92-87A5-23592C00770D}" name="Inferred design" dataDxfId="43"/>
+    <tableColumn id="16" xr3:uid="{01B4398B-886B-4B39-9F7C-BB3550166D78}" name="Number of participants" dataDxfId="42"/>
+    <tableColumn id="17" xr3:uid="{45C5B1E8-14B1-4491-AEE9-F20EEC3E0F49}" name="Probabilistic sampling" dataDxfId="41"/>
+    <tableColumn id="19" xr3:uid="{51CA66B9-1DFA-464C-BC3B-6EA038A92C8A}" name="Grade" dataDxfId="40"/>
+    <tableColumn id="21" xr3:uid="{061D070E-4B42-4273-9AAD-4EC93B84AD81}" name="Age" dataDxfId="39"/>
+    <tableColumn id="22" xr3:uid="{31070516-608E-41E0-93C1-2CC77E80426F}" name="Language" dataDxfId="38"/>
+    <tableColumn id="23" xr3:uid="{C92854F5-2EF0-4285-B7F6-8C05B4A90195}" name="Session number" dataDxfId="37"/>
+    <tableColumn id="24" xr3:uid="{B30E45D7-CC2B-4FDC-81C4-AB4317E182CE}" name="Session duration" dataDxfId="36"/>
+    <tableColumn id="25" xr3:uid="{19C302C0-56F0-45E0-95EE-BCBDAF18F282}" name="sessions frequency" dataDxfId="35"/>
+    <tableColumn id="26" xr3:uid="{ACEA4A35-6C0A-4701-8F70-24864DBA8770}" name="Modality" dataDxfId="34"/>
+    <tableColumn id="27" xr3:uid="{A06FDE04-A553-4BEF-995A-31322B29A28C}" name="Participants in group modality" dataDxfId="33"/>
+    <tableColumn id="28" xr3:uid="{0FED9BC8-7DB8-4F8E-B677-DADF5940B6CC}" name="Supervision" dataDxfId="32"/>
+    <tableColumn id="29" xr3:uid="{4D548382-0ABC-4BD6-9A3D-78FCE85DCBC1}" name="Intervention name" dataDxfId="31"/>
+    <tableColumn id="30" xr3:uid="{63FCD5C3-B077-493B-B321-B0604366EB96}" name="Instruments to measure cognition" dataDxfId="30"/>
+    <tableColumn id="31" xr3:uid="{E3A52C0B-9BE7-4A14-93E7-C4247CE91B90}" name="Instruments to measure reading skills" dataDxfId="29"/>
+    <tableColumn id="32" xr3:uid="{0D56973D-C88D-40FE-A90F-B0AFB213AFDF}" name="Random assignment" dataDxfId="28"/>
+    <tableColumn id="33" xr3:uid="{ECFDDC08-D3B7-4CF9-AF2D-BA1AAE9641F6}" name="Assessment counterbalancing" dataDxfId="27"/>
+    <tableColumn id="34" xr3:uid="{EE5CE2B4-6D44-44A0-BC90-566EB9520766}" name="Variables for group balance" dataDxfId="26"/>
+    <tableColumn id="37" xr3:uid="{C28C160E-D7AE-41F1-9FB7-C3E66D709720}" name="Other methodological controls" dataDxfId="25"/>
+    <tableColumn id="38" xr3:uid="{2EA382FB-29FE-4AAB-A2D4-55C13414BFF5}" name="Descriptive statistics provided" dataDxfId="24"/>
+    <tableColumn id="39" xr3:uid="{09505FCD-0E9E-4883-A35E-0564AA34BA56}" name="Mean/Median" dataDxfId="23"/>
+    <tableColumn id="40" xr3:uid="{484DDF92-F6A0-4359-8958-DC5B1C8A3B0C}" name="Standard deviation" dataDxfId="22"/>
+    <tableColumn id="41" xr3:uid="{55D2984D-1B81-4C5D-887F-785B42549436}" name="Mean confidence interval" dataDxfId="21"/>
+    <tableColumn id="42" xr3:uid="{1C5ABDAC-5E8F-4586-AF3F-5CE38E434290}" name="Other descriptive statistics" dataDxfId="20"/>
+    <tableColumn id="57" xr3:uid="{C48DCD7B-4527-4E53-A3F7-E60E0ECEF558}" name="Comments about descriptive statistics" dataDxfId="19"/>
+    <tableColumn id="44" xr3:uid="{7A4931EC-DAB2-43FD-9563-B41C63AF994C}" name="Inferential statistics" dataDxfId="18"/>
+    <tableColumn id="45" xr3:uid="{04FD368E-6727-4A16-B432-6055946ADB4E}" name="Covariate" dataDxfId="17"/>
+    <tableColumn id="46" xr3:uid="{002B09FC-42A5-4B9E-B00B-4247469ED640}" name="Specific p-value provided" dataDxfId="16"/>
+    <tableColumn id="47" xr3:uid="{2491D4F3-A98E-4ED6-9CC0-5BEBA0AED5A2}" name="Effect size provided" dataDxfId="15"/>
+    <tableColumn id="48" xr3:uid="{ED100DE6-09FF-4604-99D6-73681EB7237F}" name="Mean difference confidence interval" dataDxfId="14"/>
+    <tableColumn id="49" xr3:uid="{51DB6773-4D14-4AE1-9DA6-3C452E8BD712}" name="Other statistical controls" dataDxfId="13"/>
+    <tableColumn id="58" xr3:uid="{5B74B444-7863-49DC-BECA-49FEE05F9984}" name="Comments inferential statistics" dataDxfId="12"/>
+    <tableColumn id="50" xr3:uid="{E36D3572-9344-404D-AEED-4C18E7A993EF}" name="Improved cognitive processes" dataDxfId="11"/>
+    <tableColumn id="51" xr3:uid="{2B520559-FCB3-4512-B091-68EA56AAEE21}" name="Cognitive processes that did not improve" dataDxfId="10"/>
+    <tableColumn id="52" xr3:uid="{1EA75320-37D8-4F15-940E-B6A10594C3A3}" name="Effect size cognition" dataDxfId="9"/>
+    <tableColumn id="59" xr3:uid="{D5BEAA29-1A8C-40F5-9AC8-5637860CE237}" name="Comments effect on cognition" dataDxfId="8"/>
+    <tableColumn id="3" xr3:uid="{05BA5D65-9865-E24C-8C24-D3F101DAAF39}" name="Improved reading skills" dataDxfId="7"/>
+    <tableColumn id="53" xr3:uid="{C933BD5B-B918-4F2D-B8F7-CD8E7A132A17}" name="Improved reading skills_coded" dataDxfId="6"/>
+    <tableColumn id="4" xr3:uid="{7FF23964-25F2-9E4E-A060-98AF4F47BE84}" name="Reading skills no improvement" dataDxfId="5"/>
+    <tableColumn id="54" xr3:uid="{F39DD7A1-CBC3-4AF0-B362-68FFD32F347B}" name="Reading skills no improvement_coded" dataDxfId="2"/>
+    <tableColumn id="55" xr3:uid="{A6F391AD-5850-47C2-9D08-4CFA06D01676}" name="Effect size reading skills" dataDxfId="0"/>
+    <tableColumn id="7" xr3:uid="{8C25F0B5-667D-0C43-963E-42642928D327}" name="Effect size classification" dataDxfId="1"/>
+    <tableColumn id="60" xr3:uid="{6050F297-C3B7-4DDE-A740-5139D8EAF8F5}" name="Comments effect on reading skills" dataDxfId="4"/>
+    <tableColumn id="61" xr3:uid="{C3B05082-6C97-4BD7-B093-5FB9EEC21E36}" name="General comments" dataDxfId="3"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2686,10 +2743,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DCC8F8-9AF7-4852-993C-1C43D0DE4DF4}">
-  <dimension ref="A1:BE23"/>
+  <dimension ref="A1:BF23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AY1" zoomScale="200" zoomScaleNormal="75" workbookViewId="0">
-      <selection activeCell="AY1" sqref="AY1:AY1048576"/>
+    <sheetView tabSelected="1" topLeftCell="AY12" zoomScale="200" zoomScaleNormal="75" workbookViewId="0">
+      <selection activeCell="AZ25" sqref="AZ25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2734,182 +2791,186 @@
     <col min="48" max="48" width="47.83203125" style="2" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="28.5" style="2" customWidth="1"/>
     <col min="50" max="50" width="52.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="51" max="51" width="63.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="52" max="52" width="25.33203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="53" max="53" width="255.83203125" style="13" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="8.83203125" style="13"/>
-    <col min="55" max="55" width="68.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="56" max="57" width="28.5" style="2" customWidth="1"/>
-    <col min="58" max="58" width="8.83203125" style="13"/>
-    <col min="59" max="59" width="9" style="13" customWidth="1"/>
-    <col min="60" max="16384" width="8.83203125" style="13"/>
+    <col min="51" max="51" width="39" style="15" customWidth="1"/>
+    <col min="52" max="52" width="15.5" style="2" customWidth="1"/>
+    <col min="53" max="53" width="25.33203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="255.83203125" style="13" bestFit="1" customWidth="1"/>
+    <col min="55" max="55" width="8.83203125" style="13"/>
+    <col min="56" max="56" width="68.83203125" style="2" bestFit="1" customWidth="1"/>
+    <col min="57" max="58" width="28.5" style="2" customWidth="1"/>
+    <col min="59" max="59" width="8.83203125" style="13"/>
+    <col min="60" max="60" width="9" style="13" customWidth="1"/>
+    <col min="61" max="16384" width="8.83203125" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" ht="17" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:58" ht="17" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>213</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>215</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>216</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>217</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="H1" s="2" t="s">
-        <v>369</v>
-      </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
+        <v>278</v>
+      </c>
+      <c r="K1" s="2" t="s">
         <v>219</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>279</v>
-      </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>220</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>221</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>223</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>224</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>225</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>226</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="S1" s="2" t="s">
+      <c r="T1" s="2" t="s">
         <v>228</v>
       </c>
-      <c r="T1" s="2" t="s">
+      <c r="U1" s="2" t="s">
         <v>229</v>
       </c>
-      <c r="U1" s="2" t="s">
+      <c r="V1" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="V1" s="2" t="s">
+      <c r="W1" s="2" t="s">
         <v>231</v>
       </c>
-      <c r="W1" s="2" t="s">
+      <c r="X1" s="2" t="s">
         <v>232</v>
       </c>
-      <c r="X1" s="2" t="s">
+      <c r="Y1" s="2" t="s">
         <v>233</v>
       </c>
-      <c r="Y1" s="2" t="s">
+      <c r="Z1" s="2" t="s">
         <v>234</v>
       </c>
-      <c r="Z1" s="2" t="s">
+      <c r="AA1" s="2" t="s">
         <v>235</v>
       </c>
-      <c r="AA1" s="2" t="s">
+      <c r="AB1" s="2" t="s">
         <v>236</v>
       </c>
-      <c r="AB1" s="2" t="s">
+      <c r="AC1" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="AC1" s="2" t="s">
+      <c r="AD1" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="AD1" s="2" t="s">
+      <c r="AE1" s="2" t="s">
         <v>239</v>
       </c>
-      <c r="AE1" s="2" t="s">
+      <c r="AF1" s="2" t="s">
         <v>240</v>
       </c>
-      <c r="AF1" s="2" t="s">
+      <c r="AG1" s="2" t="s">
+        <v>246</v>
+      </c>
+      <c r="AH1" s="2" t="s">
         <v>241</v>
       </c>
-      <c r="AG1" s="2" t="s">
+      <c r="AI1" s="2" t="s">
+        <v>242</v>
+      </c>
+      <c r="AJ1" s="2" t="s">
+        <v>243</v>
+      </c>
+      <c r="AK1" s="2" t="s">
+        <v>244</v>
+      </c>
+      <c r="AL1" s="2" t="s">
+        <v>311</v>
+      </c>
+      <c r="AM1" s="2" t="s">
+        <v>245</v>
+      </c>
+      <c r="AN1" s="2" t="s">
         <v>247</v>
       </c>
-      <c r="AH1" s="2" t="s">
-        <v>242</v>
-      </c>
-      <c r="AI1" s="2" t="s">
-        <v>243</v>
-      </c>
-      <c r="AJ1" s="2" t="s">
-        <v>244</v>
-      </c>
-      <c r="AK1" s="2" t="s">
-        <v>245</v>
-      </c>
-      <c r="AL1" s="2" t="s">
-        <v>312</v>
-      </c>
-      <c r="AM1" s="2" t="s">
-        <v>246</v>
-      </c>
-      <c r="AN1" s="2" t="s">
+      <c r="AO1" s="2" t="s">
         <v>248</v>
       </c>
-      <c r="AO1" s="2" t="s">
+      <c r="AP1" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="AP1" s="2" t="s">
+      <c r="AQ1" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="AQ1" s="2" t="s">
+      <c r="AR1" s="2" t="s">
         <v>251</v>
       </c>
-      <c r="AR1" s="2" t="s">
+      <c r="AS1" s="2" t="s">
         <v>252</v>
       </c>
-      <c r="AS1" s="2" t="s">
+      <c r="AT1" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="AU1" s="2" t="s">
         <v>253</v>
       </c>
-      <c r="AT1" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="AU1" s="2" t="s">
+      <c r="AV1" s="2" t="s">
+        <v>334</v>
+      </c>
+      <c r="AW1" s="2" t="s">
         <v>254</v>
       </c>
-      <c r="AV1" s="2" t="s">
+      <c r="AX1" s="2" t="s">
         <v>335</v>
       </c>
-      <c r="AW1" s="2" t="s">
+      <c r="AY1" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="AX1" s="2" t="s">
-        <v>336</v>
-      </c>
-      <c r="AY1" s="2" t="s">
+      <c r="AZ1" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="BA1" s="2" t="s">
         <v>256</v>
       </c>
-      <c r="AZ1" s="2" t="s">
-        <v>257</v>
-      </c>
-      <c r="BA1" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="BC1" s="13"/>
+      <c r="BB1" s="2" t="s">
+        <v>200</v>
+      </c>
       <c r="BD1" s="13"/>
       <c r="BE1" s="13"/>
+      <c r="BF1" s="13"/>
     </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A2" s="2">
         <v>2</v>
       </c>
@@ -2929,19 +2990,19 @@
         <v>888</v>
       </c>
       <c r="G2" s="9" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>54</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K2" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>55</v>
@@ -2962,7 +3023,7 @@
         <v>40</v>
       </c>
       <c r="R2" s="5" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="S2" s="2" t="s">
         <v>97</v>
@@ -2974,7 +3035,7 @@
         <v>888</v>
       </c>
       <c r="V2" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="W2" s="2" t="s">
         <v>57</v>
@@ -2998,13 +3059,13 @@
         <v>888</v>
       </c>
       <c r="AD2" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE2" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF2" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG2" s="2" t="s">
         <v>14</v>
@@ -3017,19 +3078,19 @@
         <v>40</v>
       </c>
       <c r="AK2" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AL2" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AM2" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AN2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AP2" s="3" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="AQ2" s="2">
         <v>888</v>
@@ -3042,29 +3103,32 @@
       </c>
       <c r="AT2" s="3"/>
       <c r="AU2" s="9" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="AV2" s="2" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="AW2" s="9" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="AX2" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="AY2" s="3" t="s">
-        <v>188</v>
-      </c>
-      <c r="AZ2" s="3"/>
-      <c r="BA2" s="3" t="s">
-        <v>292</v>
-      </c>
-      <c r="BC2" s="13"/>
+        <v>366</v>
+      </c>
+      <c r="AY2" s="16" t="s">
+        <v>187</v>
+      </c>
+      <c r="AZ2" s="3" t="s">
+        <v>404</v>
+      </c>
+      <c r="BA2" s="3"/>
+      <c r="BB2" s="3" t="s">
+        <v>291</v>
+      </c>
       <c r="BD2" s="13"/>
       <c r="BE2" s="13"/>
+      <c r="BF2" s="13"/>
     </row>
-    <row r="3" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A3" s="2">
         <v>3</v>
       </c>
@@ -3084,16 +3148,16 @@
         <v>888</v>
       </c>
       <c r="G3" s="9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="I3" s="2" t="s">
         <v>44</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
       <c r="K3" s="3" t="s">
         <v>14</v>
@@ -3102,7 +3166,7 @@
         <v>45</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N3" s="3" t="s">
         <v>37</v>
@@ -3117,19 +3181,19 @@
         <v>97</v>
       </c>
       <c r="R3" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S3" s="2">
         <v>5</v>
       </c>
       <c r="T3" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="U3" s="2" t="s">
         <v>97</v>
       </c>
       <c r="V3" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W3" s="2" t="s">
         <v>46</v>
@@ -3138,28 +3202,28 @@
         <v>888</v>
       </c>
       <c r="Y3" s="2" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="Z3" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AA3" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AB3" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AC3" s="2">
         <v>888</v>
       </c>
       <c r="AD3" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE3" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF3" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG3" s="2" t="s">
         <v>14</v>
@@ -3172,10 +3236,10 @@
         <v>40</v>
       </c>
       <c r="AK3" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AL3" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AM3" s="2" t="s">
         <v>14</v>
@@ -3197,31 +3261,34 @@
       </c>
       <c r="AT3" s="3"/>
       <c r="AU3" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AV3" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AW3" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="AX3" s="2" t="s">
+        <v>333</v>
+      </c>
+      <c r="AY3" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="AV3" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AW3" s="9" t="s">
-        <v>359</v>
-      </c>
-      <c r="AX3" s="2" t="s">
-        <v>334</v>
-      </c>
-      <c r="AY3" s="3" t="s">
-        <v>200</v>
-      </c>
       <c r="AZ3" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="BA3" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="BA3" s="3" t="s">
-        <v>187</v>
-      </c>
-      <c r="BC3" s="13"/>
+      <c r="BB3" s="3" t="s">
+        <v>186</v>
+      </c>
       <c r="BD3" s="13"/>
       <c r="BE3" s="13"/>
+      <c r="BF3" s="13"/>
     </row>
-    <row r="4" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A4" s="2">
         <v>4</v>
       </c>
@@ -3241,19 +3308,19 @@
         <v>888</v>
       </c>
       <c r="G4" s="9" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="I4" s="2" t="s">
         <v>64</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>65</v>
@@ -3262,7 +3329,7 @@
         <v>14</v>
       </c>
       <c r="N4" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>27</v>
@@ -3286,7 +3353,7 @@
         <v>888</v>
       </c>
       <c r="V4" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W4" s="2" t="s">
         <v>68</v>
@@ -3298,7 +3365,7 @@
         <v>69</v>
       </c>
       <c r="Z4" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AA4" s="2" t="s">
         <v>14</v>
@@ -3329,13 +3396,13 @@
         <v>40</v>
       </c>
       <c r="AK4" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AL4" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AM4" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AN4" s="2" t="s">
         <v>14</v>
@@ -3354,36 +3421,39 @@
       </c>
       <c r="AT4" s="3"/>
       <c r="AU4" s="9" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="AV4" s="2" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="AW4" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AX4" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AY4" s="3" t="s">
-        <v>400</v>
+        <v>198</v>
+      </c>
+      <c r="AY4" s="16" t="s">
+        <v>399</v>
       </c>
       <c r="AZ4" s="3" t="s">
-        <v>394</v>
+        <v>407</v>
       </c>
       <c r="BA4" s="3" t="s">
+        <v>393</v>
+      </c>
+      <c r="BB4" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="BC4" s="13"/>
       <c r="BD4" s="13"/>
       <c r="BE4" s="13"/>
+      <c r="BF4" s="13"/>
     </row>
-    <row r="5" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" s="2">
         <v>5</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>16</v>
@@ -3398,25 +3468,25 @@
         <v>888</v>
       </c>
       <c r="G5" s="9" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="H5" s="8" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="I5" s="2" t="s">
         <v>74</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K5" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L5" s="3" t="s">
         <v>75</v>
       </c>
       <c r="M5" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="N5" s="3" t="s">
         <v>76</v>
@@ -3443,7 +3513,7 @@
         <v>888</v>
       </c>
       <c r="V5" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W5" s="2" t="s">
         <v>79</v>
@@ -3455,25 +3525,25 @@
         <v>80</v>
       </c>
       <c r="Z5" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AA5" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AB5" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AC5" s="2">
         <v>888</v>
       </c>
       <c r="AD5" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE5" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF5" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG5" s="2" t="s">
         <v>14</v>
@@ -3486,13 +3556,13 @@
         <v>40</v>
       </c>
       <c r="AK5" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AL5" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AM5" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AN5" s="2" t="s">
         <v>14</v>
@@ -3508,30 +3578,33 @@
         <v>888</v>
       </c>
       <c r="AT5" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AU5" s="9" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="AV5" s="2" t="s">
+        <v>363</v>
+      </c>
+      <c r="AW5" s="9" t="s">
+        <v>360</v>
+      </c>
+      <c r="AX5" s="2" t="s">
         <v>364</v>
       </c>
-      <c r="AW5" s="9" t="s">
-        <v>361</v>
-      </c>
-      <c r="AX5" s="2" t="s">
-        <v>365</v>
-      </c>
-      <c r="AY5" s="2" t="s">
-        <v>401</v>
-      </c>
-      <c r="AZ5" s="3"/>
+      <c r="AY5" s="15" t="s">
+        <v>400</v>
+      </c>
+      <c r="AZ5" s="2" t="s">
+        <v>408</v>
+      </c>
       <c r="BA5" s="3"/>
-      <c r="BC5" s="13"/>
+      <c r="BB5" s="3"/>
       <c r="BD5" s="13"/>
       <c r="BE5" s="13"/>
+      <c r="BF5" s="13"/>
     </row>
-    <row r="6" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:58" ht="51" x14ac:dyDescent="0.2">
       <c r="A6" s="2">
         <v>6</v>
       </c>
@@ -3545,22 +3618,22 @@
         <v>83</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F6" s="2">
         <v>888</v>
       </c>
       <c r="G6" s="9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="H6" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>84</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K6" s="3" t="s">
         <v>14</v>
@@ -3572,7 +3645,7 @@
         <v>14</v>
       </c>
       <c r="N6" s="4" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="O6" s="3">
         <v>7</v>
@@ -3590,13 +3663,13 @@
         <v>37</v>
       </c>
       <c r="T6" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="U6" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="V6" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W6" s="2" t="s">
         <v>79</v>
@@ -3608,25 +3681,25 @@
         <v>88</v>
       </c>
       <c r="Z6" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AA6" s="2">
         <v>888</v>
       </c>
       <c r="AB6" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AC6" s="2" t="s">
         <v>89</v>
       </c>
       <c r="AD6" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE6" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF6" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG6" s="2" t="s">
         <v>14</v>
@@ -3639,13 +3712,13 @@
         <v>91</v>
       </c>
       <c r="AK6" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AL6" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AM6" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AN6" s="2" t="s">
         <v>14</v>
@@ -3661,32 +3734,35 @@
         <v>888</v>
       </c>
       <c r="AT6" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AU6" s="9" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="AV6" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AW6" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AX6" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AY6" s="3" t="s">
-        <v>399</v>
-      </c>
-      <c r="AZ6" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="BA6" s="3"/>
-      <c r="BC6" s="13"/>
+        <v>198</v>
+      </c>
+      <c r="AY6" s="16" t="s">
+        <v>398</v>
+      </c>
+      <c r="AZ6" s="16" t="s">
+        <v>413</v>
+      </c>
+      <c r="BA6" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="BB6" s="3"/>
       <c r="BD6" s="13"/>
       <c r="BE6" s="13"/>
+      <c r="BF6" s="13"/>
     </row>
-    <row r="7" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A7" s="2">
         <v>7</v>
       </c>
@@ -3697,7 +3773,7 @@
         <v>5</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>6</v>
@@ -3715,7 +3791,7 @@
         <v>95</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K7" s="3" t="s">
         <v>14</v>
@@ -3730,7 +3806,7 @@
         <v>97</v>
       </c>
       <c r="O7" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>9</v>
@@ -3739,7 +3815,7 @@
         <v>97</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="S7" s="3">
         <v>5</v>
@@ -3751,7 +3827,7 @@
         <v>888</v>
       </c>
       <c r="V7" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W7" s="2" t="s">
         <v>12</v>
@@ -3763,7 +3839,7 @@
         <v>13</v>
       </c>
       <c r="Z7" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AA7" s="2" t="s">
         <v>14</v>
@@ -3775,13 +3851,13 @@
         <v>888</v>
       </c>
       <c r="AD7" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE7" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF7" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG7" s="2" t="s">
         <v>14</v>
@@ -3791,19 +3867,19 @@
       </c>
       <c r="AI7" s="3"/>
       <c r="AJ7" s="2" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="AK7" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AL7" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AM7" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AN7" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AP7" s="3"/>
       <c r="AQ7" s="2">
@@ -3817,29 +3893,32 @@
       </c>
       <c r="AT7" s="3"/>
       <c r="AU7" s="9" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="AV7" s="2" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="AW7" s="9" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="AX7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="AY7" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="AZ7" s="3"/>
-      <c r="BA7" s="3" t="s">
-        <v>182</v>
-      </c>
-      <c r="BC7" s="13"/>
+      <c r="AY7" s="16" t="s">
+        <v>401</v>
+      </c>
+      <c r="AZ7" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="BA7" s="3"/>
+      <c r="BB7" s="3" t="s">
+        <v>181</v>
+      </c>
       <c r="BD7" s="13"/>
       <c r="BE7" s="13"/>
+      <c r="BF7" s="13"/>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A8" s="2">
         <v>8</v>
       </c>
@@ -3859,16 +3938,16 @@
         <v>888</v>
       </c>
       <c r="G8" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="I8" s="2" t="s">
         <v>19</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K8" s="3" t="s">
         <v>14</v>
@@ -3883,13 +3962,13 @@
         <v>97</v>
       </c>
       <c r="O8" s="3" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="P8" s="2" t="s">
         <v>9</v>
       </c>
       <c r="Q8" s="3" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="R8" s="3" t="s">
         <v>67</v>
@@ -3904,43 +3983,43 @@
         <v>888</v>
       </c>
       <c r="V8" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="W8" s="2" t="s">
+        <v>298</v>
+      </c>
+      <c r="X8" s="2">
+        <v>888</v>
+      </c>
+      <c r="Y8" s="2" t="s">
+        <v>302</v>
+      </c>
+      <c r="Z8" s="2">
+        <v>888</v>
+      </c>
+      <c r="AA8" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AB8" s="2">
+        <v>888</v>
+      </c>
+      <c r="AC8" s="2">
+        <v>888</v>
+      </c>
+      <c r="AD8" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AE8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AF8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG8" s="2">
+        <v>888</v>
+      </c>
+      <c r="AH8" s="2" t="s">
         <v>260</v>
-      </c>
-      <c r="W8" s="2" t="s">
-        <v>299</v>
-      </c>
-      <c r="X8" s="2">
-        <v>888</v>
-      </c>
-      <c r="Y8" s="2" t="s">
-        <v>303</v>
-      </c>
-      <c r="Z8" s="2">
-        <v>888</v>
-      </c>
-      <c r="AA8" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="AB8" s="2">
-        <v>888</v>
-      </c>
-      <c r="AC8" s="2">
-        <v>888</v>
-      </c>
-      <c r="AD8" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="AE8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AF8" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG8" s="2">
-        <v>888</v>
-      </c>
-      <c r="AH8" s="2" t="s">
-        <v>261</v>
       </c>
       <c r="AI8" s="3" t="s">
         <v>22</v>
@@ -3974,29 +4053,32 @@
       </c>
       <c r="AT8" s="3"/>
       <c r="AU8" s="9" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="AV8" s="2" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="AW8" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AX8" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AY8" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="AX8" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AY8" s="3" t="s">
-        <v>200</v>
-      </c>
       <c r="AZ8" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="BA8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="BA8" s="3"/>
-      <c r="BC8" s="13"/>
+      <c r="BB8" s="3"/>
       <c r="BD8" s="13"/>
       <c r="BE8" s="13"/>
+      <c r="BF8" s="13"/>
     </row>
-    <row r="9" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="2">
         <v>9</v>
       </c>
@@ -4010,13 +4092,13 @@
         <v>25</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="F9" s="2">
         <v>888</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="H9" s="8" t="s">
         <v>7</v>
@@ -4025,7 +4107,7 @@
         <v>26</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K9" s="3" t="s">
         <v>14</v>
@@ -4040,7 +4122,7 @@
         <v>97</v>
       </c>
       <c r="O9" s="4" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="P9" s="2" t="s">
         <v>9</v>
@@ -4052,16 +4134,16 @@
         <v>27</v>
       </c>
       <c r="S9" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T9" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="U9" s="3" t="s">
         <v>21</v>
       </c>
       <c r="V9" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W9" s="2" t="s">
         <v>28</v>
@@ -4070,7 +4152,7 @@
         <v>888</v>
       </c>
       <c r="Y9" s="2" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="Z9" s="2" t="s">
         <v>14</v>
@@ -4085,10 +4167,10 @@
         <v>888</v>
       </c>
       <c r="AD9" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE9" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF9" s="2" t="s">
         <v>14</v>
@@ -4097,10 +4179,10 @@
         <v>888</v>
       </c>
       <c r="AH9" s="2" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="AI9" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AJ9" s="2">
         <v>888</v>
@@ -4118,7 +4200,7 @@
         <v>14</v>
       </c>
       <c r="AP9" s="3" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="AQ9" s="2">
         <v>888</v>
@@ -4130,34 +4212,37 @@
         <v>888</v>
       </c>
       <c r="AT9" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AU9" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AV9" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AW9" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AX9" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AY9" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="AV9" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AW9" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AX9" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AY9" s="3" t="s">
-        <v>200</v>
-      </c>
       <c r="AZ9" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="BA9" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="BA9" s="3" t="s">
+      <c r="BB9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="BC9" s="13"/>
       <c r="BD9" s="13"/>
       <c r="BE9" s="13"/>
+      <c r="BF9" s="13"/>
     </row>
-    <row r="10" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A10" s="2">
         <v>10</v>
       </c>
@@ -4171,22 +4256,22 @@
         <v>94</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="F10" s="2">
         <v>888</v>
       </c>
       <c r="G10" s="9" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="H10" s="8" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>95</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K10" s="3" t="s">
         <v>14</v>
@@ -4198,10 +4283,10 @@
         <v>14</v>
       </c>
       <c r="N10" s="3" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="O10" s="4" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="P10" s="2" t="s">
         <v>9</v>
@@ -4222,10 +4307,10 @@
         <v>888</v>
       </c>
       <c r="V10" s="2" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
       <c r="W10" s="2" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
       <c r="X10" s="2">
         <v>888</v>
@@ -4234,7 +4319,7 @@
         <v>98</v>
       </c>
       <c r="Z10" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AA10" s="2" t="s">
         <v>14</v>
@@ -4246,13 +4331,13 @@
         <v>888</v>
       </c>
       <c r="AD10" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE10" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF10" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG10" s="2" t="s">
         <v>14</v>
@@ -4265,13 +4350,13 @@
         <v>40</v>
       </c>
       <c r="AK10" s="2" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="AL10" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AM10" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AN10" s="2" t="s">
         <v>14</v>
@@ -4289,30 +4374,33 @@
         <v>888</v>
       </c>
       <c r="AT10" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AU10" s="9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="AV10" s="2" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="AW10" s="9" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="AX10" s="2" t="s">
-        <v>366</v>
-      </c>
-      <c r="AY10" s="3" t="s">
-        <v>403</v>
-      </c>
-      <c r="AZ10" s="3"/>
+        <v>365</v>
+      </c>
+      <c r="AY10" s="16" t="s">
+        <v>402</v>
+      </c>
+      <c r="AZ10" s="3" t="s">
+        <v>411</v>
+      </c>
       <c r="BA10" s="3"/>
-      <c r="BC10" s="13"/>
+      <c r="BB10" s="3"/>
       <c r="BD10" s="13"/>
       <c r="BE10" s="13"/>
+      <c r="BF10" s="13"/>
     </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>11</v>
       </c>
@@ -4326,22 +4414,22 @@
         <v>33</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="F11" s="2">
         <v>888</v>
       </c>
       <c r="G11" s="9" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>34</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K11" s="3" t="s">
         <v>14</v>
@@ -4353,7 +4441,7 @@
         <v>14</v>
       </c>
       <c r="N11" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O11" s="3" t="s">
         <v>97</v>
@@ -4371,13 +4459,13 @@
         <v>3</v>
       </c>
       <c r="T11" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="U11" s="3" t="s">
         <v>37</v>
       </c>
       <c r="V11" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W11" s="2" t="s">
         <v>38</v>
@@ -4389,10 +4477,10 @@
         <v>39</v>
       </c>
       <c r="Z11" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AA11" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AB11" s="2">
         <v>888</v>
@@ -4401,13 +4489,13 @@
         <v>888</v>
       </c>
       <c r="AD11" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE11" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF11" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG11" s="2" t="s">
         <v>14</v>
@@ -4420,16 +4508,16 @@
         <v>40</v>
       </c>
       <c r="AK11" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AL11" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AM11" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AN11" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AP11" s="3"/>
       <c r="AQ11" s="2">
@@ -4442,35 +4530,38 @@
         <v>888</v>
       </c>
       <c r="AT11" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AU11" s="9" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="AV11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="AW11" s="9" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="AX11" s="2" t="s">
-        <v>367</v>
-      </c>
-      <c r="AY11" s="3" t="s">
-        <v>204</v>
-      </c>
-      <c r="AZ11" s="3"/>
+        <v>366</v>
+      </c>
+      <c r="AY11" s="16" t="s">
+        <v>203</v>
+      </c>
+      <c r="AZ11" s="3" t="s">
+        <v>407</v>
+      </c>
       <c r="BA11" s="3"/>
-      <c r="BC11" s="13"/>
+      <c r="BB11" s="3"/>
       <c r="BD11" s="13"/>
       <c r="BE11" s="13"/>
+      <c r="BF11" s="13"/>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A12" s="2">
         <v>12</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C12" s="3" t="s">
         <v>93</v>
@@ -4479,22 +4570,22 @@
         <v>100</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="F12" s="2">
         <v>888</v>
       </c>
       <c r="G12" s="9" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="H12" s="10" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="I12" s="2" t="s">
         <v>84</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="K12" s="3" t="s">
         <v>14</v>
@@ -4527,22 +4618,22 @@
         <v>11</v>
       </c>
       <c r="U12" s="4" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="V12" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W12" s="2" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="X12" s="2">
         <v>888</v>
       </c>
       <c r="Y12" s="2" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="Z12" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AA12" s="2" t="s">
         <v>14</v>
@@ -4554,35 +4645,35 @@
         <v>888</v>
       </c>
       <c r="AD12" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE12" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF12" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG12" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AH12" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AI12" s="3"/>
       <c r="AJ12" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AK12" s="2" t="s">
         <v>104</v>
       </c>
       <c r="AL12" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AM12" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AN12" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AP12" s="3" t="s">
         <v>105</v>
@@ -4597,34 +4688,37 @@
         <v>888</v>
       </c>
       <c r="AT12" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AU12" s="9" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AV12" s="2" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="AW12" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AX12" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AY12" s="3" t="s">
-        <v>189</v>
+        <v>198</v>
+      </c>
+      <c r="AY12" s="16" t="s">
+        <v>188</v>
       </c>
       <c r="AZ12" s="3" t="s">
+        <v>406</v>
+      </c>
+      <c r="BA12" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="BA12" s="3" t="s">
+      <c r="BB12" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="BC12" s="13"/>
       <c r="BD12" s="13"/>
       <c r="BE12" s="13"/>
+      <c r="BF12" s="13"/>
     </row>
-    <row r="13" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A13" s="2">
         <v>13</v>
       </c>
@@ -4638,22 +4732,22 @@
         <v>109</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F13" s="2">
         <v>888</v>
       </c>
       <c r="G13" s="9" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="H13" s="8" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="I13" s="2" t="s">
         <v>110</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K13" s="3" t="s">
         <v>14</v>
@@ -4689,37 +4783,37 @@
         <v>888</v>
       </c>
       <c r="V13" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W13" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="X13" s="2">
         <v>888</v>
       </c>
       <c r="Y13" s="2" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="Z13" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AA13" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AB13" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AC13" s="2">
         <v>888</v>
       </c>
       <c r="AD13" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE13" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF13" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG13" s="2" t="s">
         <v>14</v>
@@ -4732,13 +4826,13 @@
         <v>91</v>
       </c>
       <c r="AK13" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AL13" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AM13" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AN13" s="2" t="s">
         <v>14</v>
@@ -4755,27 +4849,30 @@
       </c>
       <c r="AT13" s="3"/>
       <c r="AU13" s="9" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="AV13" s="2" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="AW13" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AX13" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AY13" s="3" t="s">
-        <v>206</v>
-      </c>
-      <c r="AZ13" s="3"/>
+        <v>198</v>
+      </c>
+      <c r="AY13" s="16" t="s">
+        <v>205</v>
+      </c>
+      <c r="AZ13" s="3" t="s">
+        <v>407</v>
+      </c>
       <c r="BA13" s="3"/>
-      <c r="BC13" s="13"/>
+      <c r="BB13" s="3"/>
       <c r="BD13" s="13"/>
       <c r="BE13" s="13"/>
+      <c r="BF13" s="13"/>
     </row>
-    <row r="14" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A14" s="2">
         <v>14</v>
       </c>
@@ -4795,7 +4892,7 @@
         <v>888</v>
       </c>
       <c r="G14" s="9" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="H14" s="11" t="s">
         <v>7</v>
@@ -4804,7 +4901,7 @@
         <v>117</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="K14" s="3" t="s">
         <v>14</v>
@@ -4816,10 +4913,10 @@
         <v>14</v>
       </c>
       <c r="N14" s="3" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="O14" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P14" s="2" t="s">
         <v>9</v>
@@ -4834,16 +4931,16 @@
         <v>3</v>
       </c>
       <c r="T14" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="U14" s="3" t="s">
         <v>20</v>
       </c>
       <c r="V14" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W14" s="2" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
       <c r="X14" s="2">
         <v>888</v>
@@ -4864,19 +4961,19 @@
         <v>888</v>
       </c>
       <c r="AD14" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AE14" s="2" t="s">
+        <v>183</v>
+      </c>
+      <c r="AF14" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="AG14" s="2">
+        <v>888</v>
+      </c>
+      <c r="AH14" s="2" t="s">
         <v>184</v>
-      </c>
-      <c r="AE14" s="2" t="s">
-        <v>184</v>
-      </c>
-      <c r="AF14" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG14" s="2">
-        <v>888</v>
-      </c>
-      <c r="AH14" s="2" t="s">
-        <v>185</v>
       </c>
       <c r="AI14" s="3"/>
       <c r="AJ14" s="2">
@@ -4905,34 +5002,37 @@
         <v>888</v>
       </c>
       <c r="AT14" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AU14" s="9" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="AV14" s="2" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="AW14" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AX14" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AY14" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="AX14" s="2" t="s">
+      <c r="AZ14" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="BA14" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="AY14" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AZ14" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="BA14" s="3" t="s">
+      <c r="BB14" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="BC14" s="13"/>
       <c r="BD14" s="13"/>
       <c r="BE14" s="13"/>
+      <c r="BF14" s="13"/>
     </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A15" s="2">
         <v>15</v>
       </c>
@@ -4943,25 +5043,25 @@
         <v>114</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="F15" s="2">
         <v>888</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>120</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K15" s="3" t="s">
         <v>14</v>
@@ -4991,16 +5091,16 @@
         <v>37</v>
       </c>
       <c r="T15" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="U15" s="3" t="s">
         <v>97</v>
       </c>
       <c r="V15" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W15" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="X15" s="2">
         <v>888</v>
@@ -5009,7 +5109,7 @@
         <v>122</v>
       </c>
       <c r="Z15" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AA15" s="2" t="s">
         <v>14</v>
@@ -5021,10 +5121,10 @@
         <v>888</v>
       </c>
       <c r="AD15" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE15" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF15" s="2" t="s">
         <v>14</v>
@@ -5040,13 +5140,13 @@
         <v>91</v>
       </c>
       <c r="AK15" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AL15" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AM15" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AN15" s="2" t="s">
         <v>14</v>
@@ -5063,29 +5163,32 @@
       </c>
       <c r="AT15" s="3"/>
       <c r="AU15" s="9" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="AV15" s="2" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="AW15" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AX15" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AY15" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="AZ15" s="3"/>
-      <c r="BA15" s="3" t="s">
-        <v>179</v>
-      </c>
-      <c r="BC15" s="13"/>
+        <v>198</v>
+      </c>
+      <c r="AY15" s="16" t="s">
+        <v>396</v>
+      </c>
+      <c r="AZ15" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="BA15" s="3"/>
+      <c r="BB15" s="3" t="s">
+        <v>178</v>
+      </c>
       <c r="BD15" s="13"/>
       <c r="BE15" s="13"/>
+      <c r="BF15" s="13"/>
     </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A16" s="2">
         <v>16</v>
       </c>
@@ -5096,7 +5199,7 @@
         <v>114</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>123</v>
@@ -5105,16 +5208,16 @@
         <v>888</v>
       </c>
       <c r="G16" s="9" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="I16" s="2" t="s">
         <v>124</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K16" s="3" t="s">
         <v>14</v>
@@ -5126,7 +5229,7 @@
         <v>14</v>
       </c>
       <c r="N16" s="4" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="O16" s="3">
         <v>6</v>
@@ -5144,22 +5247,22 @@
         <v>37</v>
       </c>
       <c r="T16" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="U16" s="3" t="s">
         <v>97</v>
       </c>
       <c r="V16" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W16" s="2" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="X16" s="2">
         <v>888</v>
       </c>
       <c r="Y16" s="2" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="Z16" s="2" t="s">
         <v>14</v>
@@ -5168,19 +5271,19 @@
         <v>14</v>
       </c>
       <c r="AB16" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AC16" s="2">
         <v>888</v>
       </c>
       <c r="AD16" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE16" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF16" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG16" s="2" t="s">
         <v>14</v>
@@ -5193,13 +5296,13 @@
         <v>91</v>
       </c>
       <c r="AK16" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AL16" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AM16" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AN16" s="2" t="s">
         <v>14</v>
@@ -5216,29 +5319,32 @@
       </c>
       <c r="AT16" s="3"/>
       <c r="AU16" s="9" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="AV16" s="2" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="AW16" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AX16" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AY16" s="3" t="s">
-        <v>207</v>
-      </c>
-      <c r="AZ16" s="3"/>
-      <c r="BA16" s="3" t="s">
-        <v>180</v>
-      </c>
-      <c r="BC16" s="13"/>
+        <v>198</v>
+      </c>
+      <c r="AY16" s="16" t="s">
+        <v>206</v>
+      </c>
+      <c r="AZ16" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="BA16" s="3"/>
+      <c r="BB16" s="3" t="s">
+        <v>179</v>
+      </c>
       <c r="BD16" s="13"/>
       <c r="BE16" s="13"/>
+      <c r="BF16" s="13"/>
     </row>
-    <row r="17" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A17" s="2">
         <v>17</v>
       </c>
@@ -5252,25 +5358,25 @@
         <v>127</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="F17" s="2">
         <v>888</v>
       </c>
       <c r="G17" s="9" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>128</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="L17" s="3" t="s">
         <v>129</v>
@@ -5282,7 +5388,7 @@
         <v>20</v>
       </c>
       <c r="O17" s="4" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="P17" s="2" t="s">
         <v>9</v>
@@ -5291,28 +5397,28 @@
         <v>60</v>
       </c>
       <c r="R17" s="4" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S17" s="3">
         <v>5</v>
       </c>
       <c r="T17" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="U17" s="3" t="s">
         <v>97</v>
       </c>
       <c r="V17" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W17" s="2" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
       <c r="X17" s="2">
         <v>888</v>
       </c>
       <c r="Y17" s="2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="Z17" s="2" t="s">
         <v>14</v>
@@ -5321,19 +5427,19 @@
         <v>14</v>
       </c>
       <c r="AB17" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AC17" s="2" t="s">
         <v>130</v>
       </c>
       <c r="AD17" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE17" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF17" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG17" s="2" t="s">
         <v>14</v>
@@ -5346,10 +5452,10 @@
         <v>40</v>
       </c>
       <c r="AK17" s="2" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="AL17" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AM17" s="2" t="s">
         <v>14</v>
@@ -5370,34 +5476,35 @@
         <v>888</v>
       </c>
       <c r="AT17" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AU17" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AV17" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="AW17" s="9" t="s">
+        <v>357</v>
+      </c>
+      <c r="AX17" s="2" t="s">
+        <v>322</v>
+      </c>
+      <c r="AY17" s="16" t="s">
         <v>199</v>
       </c>
-      <c r="AV17" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AW17" s="9" t="s">
-        <v>358</v>
-      </c>
-      <c r="AX17" s="2" t="s">
-        <v>323</v>
-      </c>
-      <c r="AY17" s="3" t="s">
-        <v>200</v>
-      </c>
-      <c r="AZ17" s="3" t="s">
+      <c r="AZ17" s="3"/>
+      <c r="BA17" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="BA17" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="BC17" s="13"/>
+      <c r="BB17" s="3" t="s">
+        <v>292</v>
+      </c>
       <c r="BD17" s="13"/>
       <c r="BE17" s="13"/>
+      <c r="BF17" s="13"/>
     </row>
-    <row r="18" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="2">
         <v>18</v>
       </c>
@@ -5411,22 +5518,22 @@
         <v>134</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="F18" s="2">
         <v>888</v>
       </c>
       <c r="G18" s="9" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="H18" s="7" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>135</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="K18" s="3" t="s">
         <v>14</v>
@@ -5453,7 +5560,7 @@
         <v>10</v>
       </c>
       <c r="S18" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="T18" s="2" t="s">
         <v>11</v>
@@ -5462,7 +5569,7 @@
         <v>888</v>
       </c>
       <c r="V18" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W18" s="2" t="s">
         <v>138</v>
@@ -5507,13 +5614,13 @@
         <v>140</v>
       </c>
       <c r="AK18" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AL18" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AM18" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AN18" s="2" t="s">
         <v>14</v>
@@ -5532,29 +5639,32 @@
       </c>
       <c r="AT18" s="3"/>
       <c r="AU18" s="9" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="AV18" s="2" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="AW18" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AX18" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AY18" s="3" t="s">
-        <v>205</v>
-      </c>
-      <c r="AZ18" s="3"/>
-      <c r="BA18" s="3" t="s">
-        <v>291</v>
-      </c>
-      <c r="BC18" s="13"/>
+        <v>198</v>
+      </c>
+      <c r="AY18" s="16" t="s">
+        <v>204</v>
+      </c>
+      <c r="AZ18" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="BA18" s="3"/>
+      <c r="BB18" s="3" t="s">
+        <v>290</v>
+      </c>
       <c r="BD18" s="13"/>
       <c r="BE18" s="13"/>
+      <c r="BF18" s="13"/>
     </row>
-    <row r="19" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:58" ht="85" x14ac:dyDescent="0.2">
       <c r="A19" s="2">
         <v>19</v>
       </c>
@@ -5574,16 +5684,16 @@
         <v>888</v>
       </c>
       <c r="G19" s="9" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="H19" s="8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="I19" s="2" t="s">
         <v>146</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="K19" s="3" t="s">
         <v>14</v>
@@ -5613,13 +5723,13 @@
         <v>37</v>
       </c>
       <c r="T19" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="U19" s="3" t="s">
         <v>97</v>
       </c>
       <c r="V19" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W19" s="2" t="s">
         <v>148</v>
@@ -5628,7 +5738,7 @@
         <v>888</v>
       </c>
       <c r="Y19" s="2" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="Z19" s="2" t="s">
         <v>14</v>
@@ -5643,13 +5753,13 @@
         <v>888</v>
       </c>
       <c r="AD19" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE19" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF19" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG19" s="2" t="s">
         <v>14</v>
@@ -5658,19 +5768,19 @@
         <v>888</v>
       </c>
       <c r="AI19" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AJ19" s="2" t="s">
         <v>149</v>
       </c>
       <c r="AK19" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AL19" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AM19" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AN19" s="2" t="s">
         <v>14</v>
@@ -5688,69 +5798,72 @@
         <v>888</v>
       </c>
       <c r="AT19" s="3" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="AU19" s="9" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="AV19" s="2" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="AW19" s="9" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="AX19" s="2" t="s">
-        <v>333</v>
-      </c>
-      <c r="AY19" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="AZ19" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="AY19" s="16" t="s">
+        <v>397</v>
+      </c>
+      <c r="AZ19" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="BA19" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="BB19" s="3" t="s">
         <v>151</v>
       </c>
-      <c r="BA19" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="BC19" s="13"/>
       <c r="BD19" s="13"/>
       <c r="BE19" s="13"/>
+      <c r="BF19" s="13"/>
     </row>
-    <row r="20" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="2">
         <v>20</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C20" s="3" t="s">
         <v>61</v>
       </c>
       <c r="D20" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>273</v>
+      </c>
+      <c r="F20" s="2">
+        <v>888</v>
+      </c>
+      <c r="G20" s="9" t="s">
+        <v>383</v>
+      </c>
+      <c r="H20" s="8" t="s">
+        <v>390</v>
+      </c>
+      <c r="I20" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="E20" s="2" t="s">
-        <v>274</v>
-      </c>
-      <c r="F20" s="2">
-        <v>888</v>
-      </c>
-      <c r="G20" s="9" t="s">
-        <v>384</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>391</v>
-      </c>
-      <c r="I20" s="2" t="s">
+      <c r="J20" s="2" t="s">
+        <v>286</v>
+      </c>
+      <c r="K20" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L20" s="3" t="s">
         <v>155</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>287</v>
-      </c>
-      <c r="K20" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L20" s="3" t="s">
-        <v>156</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>14</v>
@@ -5762,13 +5875,13 @@
         <v>97</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Q20" s="3">
         <v>25</v>
       </c>
       <c r="R20" s="3" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="S20" s="3" t="s">
         <v>97</v>
@@ -5780,40 +5893,40 @@
         <v>888</v>
       </c>
       <c r="V20" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W20" s="2" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="X20" s="2">
         <v>888</v>
       </c>
       <c r="Y20" s="2" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="Z20" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AA20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AB20" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AC20" s="2">
         <v>888</v>
       </c>
       <c r="AD20" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE20" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF20" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG20" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AH20" s="2" t="s">
         <v>14</v>
@@ -5823,13 +5936,13 @@
         <v>91</v>
       </c>
       <c r="AK20" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AL20" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AM20" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AN20" s="2" t="s">
         <v>14</v>
@@ -5846,62 +5959,65 @@
       </c>
       <c r="AT20" s="3"/>
       <c r="AU20" s="9" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="AV20" s="2" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="AW20" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AX20" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AY20" s="3" t="s">
-        <v>208</v>
-      </c>
-      <c r="AZ20" s="3"/>
+        <v>198</v>
+      </c>
+      <c r="AY20" s="16" t="s">
+        <v>207</v>
+      </c>
+      <c r="AZ20" s="3" t="s">
+        <v>411</v>
+      </c>
       <c r="BA20" s="3"/>
-      <c r="BC20" s="13"/>
+      <c r="BB20" s="3"/>
       <c r="BD20" s="13"/>
       <c r="BE20" s="13"/>
+      <c r="BF20" s="13"/>
     </row>
-    <row r="21" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A21" s="2">
         <v>21</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C21" s="3" t="s">
         <v>82</v>
       </c>
       <c r="D21" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>274</v>
+      </c>
+      <c r="F21" s="2">
+        <v>888</v>
+      </c>
+      <c r="G21" s="9" t="s">
+        <v>384</v>
+      </c>
+      <c r="H21" s="12" t="s">
+        <v>391</v>
+      </c>
+      <c r="I21" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="E21" s="2" t="s">
-        <v>275</v>
-      </c>
-      <c r="F21" s="2">
-        <v>888</v>
-      </c>
-      <c r="G21" s="9" t="s">
-        <v>385</v>
-      </c>
-      <c r="H21" s="12" t="s">
-        <v>392</v>
-      </c>
-      <c r="I21" s="2" t="s">
+      <c r="J21" s="2" t="s">
+        <v>280</v>
+      </c>
+      <c r="K21" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="L21" s="3" t="s">
         <v>160</v>
-      </c>
-      <c r="J21" s="2" t="s">
-        <v>281</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>161</v>
       </c>
       <c r="M21" s="2" t="s">
         <v>14</v>
@@ -5910,7 +6026,7 @@
         <v>97</v>
       </c>
       <c r="O21" s="4" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="P21" s="2" t="s">
         <v>9</v>
@@ -5919,7 +6035,7 @@
         <v>97</v>
       </c>
       <c r="R21" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="S21" s="3">
         <v>5</v>
@@ -5931,17 +6047,17 @@
         <v>888</v>
       </c>
       <c r="V21" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W21" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="X21" s="2">
+        <v>888</v>
+      </c>
+      <c r="Y21" s="2" t="s">
         <v>163</v>
       </c>
-      <c r="X21" s="2">
-        <v>888</v>
-      </c>
-      <c r="Y21" s="2" t="s">
-        <v>164</v>
-      </c>
       <c r="Z21" s="2" t="s">
         <v>14</v>
       </c>
@@ -5955,13 +6071,13 @@
         <v>888</v>
       </c>
       <c r="AD21" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE21" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF21" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG21" s="2" t="s">
         <v>14</v>
@@ -5974,13 +6090,13 @@
         <v>91</v>
       </c>
       <c r="AK21" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AL21" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AM21" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AN21" s="2" t="s">
         <v>14</v>
@@ -5997,58 +6113,61 @@
       </c>
       <c r="AT21" s="3"/>
       <c r="AU21" s="9" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="AV21" s="2" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="AW21" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="AX21" s="2" t="s">
-        <v>199</v>
-      </c>
-      <c r="AY21" s="3" t="s">
-        <v>209</v>
-      </c>
-      <c r="AZ21" s="3"/>
-      <c r="BA21" s="3" t="s">
-        <v>288</v>
-      </c>
-      <c r="BC21" s="13"/>
+        <v>198</v>
+      </c>
+      <c r="AY21" s="16" t="s">
+        <v>208</v>
+      </c>
+      <c r="AZ21" s="3" t="s">
+        <v>412</v>
+      </c>
+      <c r="BA21" s="3"/>
+      <c r="BB21" s="3" t="s">
+        <v>287</v>
+      </c>
       <c r="BD21" s="13"/>
       <c r="BE21" s="13"/>
+      <c r="BF21" s="13"/>
     </row>
-    <row r="22" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:58" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="2">
         <v>22</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="C22" s="2">
         <v>2018</v>
       </c>
       <c r="D22" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="E22" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="E22" s="2" t="s">
-        <v>166</v>
-      </c>
       <c r="F22" s="2" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="G22" s="14" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="H22" s="6" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I22" s="2" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="J22" s="2" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="K22" s="2" t="s">
         <v>14</v>
@@ -6069,34 +6188,34 @@
         <v>9</v>
       </c>
       <c r="Q22" s="5" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="R22" s="5" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="S22" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="T22" s="2" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="U22" s="5" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="V22" s="2" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="W22" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="X22" s="2" t="s">
         <v>167</v>
       </c>
-      <c r="X22" s="2" t="s">
+      <c r="Y22" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="Y22" s="2" t="s">
-        <v>169</v>
-      </c>
       <c r="Z22" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AA22" s="2" t="s">
         <v>14</v>
@@ -6108,13 +6227,13 @@
         <v>888</v>
       </c>
       <c r="AD22" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AE22" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AF22" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AG22" s="2" t="s">
         <v>14</v>
@@ -6124,58 +6243,61 @@
       </c>
       <c r="AI22" s="2"/>
       <c r="AJ22" s="2" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="AK22" s="2" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="AL22" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AM22" s="2" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="AN22" s="2" t="s">
         <v>14</v>
       </c>
       <c r="AO22" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="AQ22" s="2" t="s">
         <v>174</v>
       </c>
-      <c r="AQ22" s="2" t="s">
+      <c r="AR22" s="2">
+        <v>888</v>
+      </c>
+      <c r="AS22" s="2" t="s">
         <v>175</v>
       </c>
-      <c r="AR22" s="2">
-        <v>888</v>
-      </c>
-      <c r="AS22" s="2" t="s">
+      <c r="AU22" s="9" t="s">
+        <v>346</v>
+      </c>
+      <c r="AV22" s="2" t="s">
+        <v>362</v>
+      </c>
+      <c r="AW22" s="9" t="s">
+        <v>358</v>
+      </c>
+      <c r="AX22" s="2" t="s">
+        <v>367</v>
+      </c>
+      <c r="AY22" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="AU22" s="9" t="s">
-        <v>347</v>
-      </c>
-      <c r="AV22" s="2" t="s">
-        <v>363</v>
-      </c>
-      <c r="AW22" s="9" t="s">
-        <v>359</v>
-      </c>
-      <c r="AX22" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="AY22" s="2" t="s">
-        <v>177</v>
-      </c>
-      <c r="AZ22" s="2"/>
+      <c r="AZ22" s="2" t="s">
+        <v>411</v>
+      </c>
       <c r="BA22" s="2"/>
       <c r="BB22" s="2"/>
-      <c r="BD22" s="13"/>
+      <c r="BC22" s="2"/>
       <c r="BE22" s="13"/>
+      <c r="BF22" s="13"/>
     </row>
-    <row r="23" spans="1:57" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:58" x14ac:dyDescent="0.2">
       <c r="A23" s="2"/>
       <c r="AI23" s="2"/>
-      <c r="AZ23" s="2"/>
       <c r="BA23" s="2"/>
+      <c r="BB23" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6187,6 +6309,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100099F4328816B724ABB65184634EDCB7A" ma:contentTypeVersion="4" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="1bd4f96a89e0bf3f95a675bb701c673a">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="17c5fd42-a044-4f07-a556-35a9304bdabd" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="0e0b4ba08ccf20d12e7907069f81316d" ns2:_="">
     <xsd:import namespace="17c5fd42-a044-4f07-a556-35a9304bdabd"/>
@@ -6332,15 +6463,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -6348,6 +6470,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81546A3-C62E-44CE-A065-5F6C0D4A2117}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D8BD45EC-7A23-43D7-AAF9-EC9E08ECF9A6}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -6366,26 +6496,18 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D81546A3-C62E-44CE-A065-5F6C0D4A2117}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{67AF54F8-9454-44E1-A274-4CE13ABA8D28}">
   <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
     <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="17c5fd42-a044-4f07-a556-35a9304bdabd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
     <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="17c5fd42-a044-4f07-a556-35a9304bdabd"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>